<commit_message>
fine i'll give up me'lucky charms
</commit_message>
<xml_diff>
--- a/Where to Eat in Triangle.xlsx
+++ b/Where to Eat in Triangle.xlsx
@@ -8,24 +8,34 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacobford/Documents/GitHub/Blog/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC0F36CF-823B-714A-93E4-2158B6B0C818}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E847681-03AE-C441-ABEC-F06AD35FEEA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="18660" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="49">
   <si>
     <t>Name</t>
   </si>
@@ -36,9 +46,6 @@
     <t>Genre</t>
   </si>
   <si>
-    <t>Lat/Long</t>
-  </si>
-  <si>
     <t>Bandito Bodega</t>
   </si>
   <si>
@@ -48,9 +55,6 @@
     <t>Japanese Fusion</t>
   </si>
   <si>
-    <t>36.07511601903717, -79.81414664232867</t>
-  </si>
-  <si>
     <t>Don't Miss:</t>
   </si>
   <si>
@@ -150,40 +154,35 @@
     <t>Chinese</t>
   </si>
   <si>
-    <t>36.00040374403168, -78.90834379629939</t>
-  </si>
-  <si>
-    <t>35.996805562745045, -78.90479608889132</t>
-  </si>
-  <si>
-    <t>35.99742132133595, -78.90123733121978</t>
-  </si>
-  <si>
-    <t>35.9975309211792, -78.90097884471247</t>
-  </si>
-  <si>
-    <t>36.08710803108532, -79.10319694471033</t>
-  </si>
-  <si>
-    <t>36.017813715073345, -78.89040490238354</t>
-  </si>
-  <si>
     <t>Don Becerra Taqueria</t>
   </si>
   <si>
     <t>Mole</t>
   </si>
   <si>
-    <t>36.02003678206182, -78.89025412030075</t>
-  </si>
-  <si>
-    <t>36.03795281969392, -78.93035484899929</t>
-  </si>
-  <si>
-    <t>35.789540832624056, -78.78018733172959</t>
-  </si>
-  <si>
-    <t>35.81937817387878, -78.82880720238848</t>
+    <t>Latitutde</t>
+  </si>
+  <si>
+    <t>Longitude</t>
+  </si>
+  <si>
+    <t>Lime and Lemon</t>
+  </si>
+  <si>
+    <t>Gobi Manchurian - Holy hell banging</t>
+  </si>
+  <si>
+    <t>Indian</t>
+  </si>
+  <si>
+    <t>Gocciolina</t>
+  </si>
+  <si>
+    <t>Italian</t>
+  </si>
+  <si>
+    <t>Chalk board menu c'mon now;
+Radicchio apetizer</t>
   </si>
 </sst>
 </file>
@@ -219,8 +218,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -501,10 +504,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -513,10 +516,9 @@
     <col min="2" max="2" width="11.83203125" customWidth="1"/>
     <col min="3" max="3" width="17.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -524,200 +526,276 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
       </c>
       <c r="E1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" s="1">
+        <v>36.075116000000001</v>
+      </c>
+      <c r="F2" s="1">
+        <v>-79.814146600000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="1">
+        <v>36.0004037</v>
+      </c>
+      <c r="F3" s="1">
+        <v>-78.908343700000003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
         <v>14</v>
       </c>
-      <c r="E3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="D4" t="s">
         <v>13</v>
       </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="E4" s="1">
+        <v>35.996805500000001</v>
+      </c>
+      <c r="F4" s="1">
+        <v>-78.904796000000005</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
         <v>16</v>
       </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="D5" t="s">
         <v>17</v>
       </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="E5" s="1">
+        <v>35.997421299999999</v>
+      </c>
+      <c r="F5" s="1">
+        <v>-78.901237300000005</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>18</v>
       </c>
-      <c r="D5" t="s">
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
         <v>19</v>
       </c>
-      <c r="E5" t="s">
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="1">
+        <v>35.997530900000001</v>
+      </c>
+      <c r="F6" s="1">
+        <v>-78.900978800000004</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="1">
+        <v>36.087108000000001</v>
+      </c>
+      <c r="F7" s="1">
+        <v>-79.1031969</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="1">
+        <v>36.017813699999998</v>
+      </c>
+      <c r="F8" s="1">
+        <v>-78.890404899999993</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="1">
+        <v>35.819378100000002</v>
+      </c>
+      <c r="F9" s="1">
+        <v>-78.8288072</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="1">
+        <v>35.789540799999997</v>
+      </c>
+      <c r="F10" s="1">
+        <v>-78.780187299999994</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="1">
+        <v>36.037952799999999</v>
+      </c>
+      <c r="F11" s="1">
+        <v>-78.930354800000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="1">
+        <v>36.020036699999999</v>
+      </c>
+      <c r="F12" s="1">
+        <v>-78.890254100000007</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="D13" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="E13" s="1">
+        <v>36.011507979731697</v>
+      </c>
+      <c r="F13" s="1">
+        <v>-78.9221750870406</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E9" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>34</v>
-      </c>
-      <c r="B10" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10" t="s">
-        <v>36</v>
-      </c>
-      <c r="D10" t="s">
-        <v>37</v>
-      </c>
-      <c r="E10" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>38</v>
-      </c>
-      <c r="B11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" t="s">
-        <v>39</v>
-      </c>
-      <c r="D11" t="s">
-        <v>40</v>
-      </c>
-      <c r="E11" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" t="s">
         <v>47</v>
       </c>
-      <c r="B12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" t="s">
-        <v>48</v>
-      </c>
-      <c r="D12" t="s">
-        <v>29</v>
-      </c>
-      <c r="E12" t="s">
-        <v>49</v>
+      <c r="E14" s="1">
+        <v>36.041552644282604</v>
+      </c>
+      <c r="F14" s="1">
+        <v>-78.928357785732501</v>
       </c>
     </row>
   </sheetData>

</xml_diff>